<commit_message>
Correction quand l'âge est désactivé
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3DB29D-645B-4FDF-B22E-E0ADE5977782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEE5677-E285-4000-B801-570275E57781}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1860" yWindow="1380" windowWidth="26640" windowHeight="13950" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>Age au camp</t>
   </si>
   <si>
-    <t>${adherent.agecamp}</t>
-  </si>
-  <si>
     <t>${adherent.ageokcamp}</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>${adherent.age}</t>
-  </si>
-  <si>
     <t>Droit à l'image OK ?</t>
   </si>
   <si>
@@ -271,6 +265,12 @@
   </si>
   <si>
     <t>Droit à l'image OK : Elle indique si le jeune peut apparaitre sur les photos ou des reportages TV par exemple.</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${adherent.agecalcule}"&gt;${adherent.age}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${adherent.agecalcule}"&gt;${adherent.agecamp}&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>
@@ -953,64 +953,64 @@
   <sheetData>
     <row r="1" spans="1:1" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1018,22 +1018,22 @@
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>32</v>
@@ -1093,16 +1093,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>15</v>
@@ -1117,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1131,25 +1131,25 @@
         <v>21</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>22</v>
@@ -1161,10 +1161,10 @@
         <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q2" t="s">
         <v>0</v>
@@ -1259,51 +1259,51 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" t="s">
         <v>54</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="s">
-        <v>56</v>
       </c>
       <c r="K2" s="1"/>
     </row>

</xml_diff>

<commit_message>
Ajout les droits (image et informations) pour jeunes et responsables #25
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\outilssgdf\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46D01BC-8895-41D2-AE45-AB8C1B3F9E83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE61738-549E-4E0E-9889-94F64B12CD3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1125" yWindow="810" windowWidth="25440" windowHeight="14565" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alertes!$A$1:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Effectifs!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Jeunes!$A$1:$N$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Jeunes!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>Branche N</t>
+  </si>
+  <si>
+    <t>Droit informations OK ?</t>
+  </si>
+  <si>
+    <t>${adherent.droitinformationsok}</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
     <cellStyle name="Filler1" xfId="1" xr:uid="{CF299C21-B143-458E-AE9E-A0A1BA0CBE68}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <color theme="0"/>
@@ -525,6 +531,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -880,93 +896,93 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="157" customWidth="1"/>
-    <col min="2" max="2" width="47.453125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
     </row>
-    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="23" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>60</v>
       </c>
@@ -982,31 +998,32 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="57.26953125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="11" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="8" style="2" customWidth="1"/>
     <col min="12" max="14" width="11" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.453125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="26" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="26" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1049,8 +1066,11 @@
       <c r="N1" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O1" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -1093,24 +1113,32 @@
       <c r="N2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N2" xr:uid="{1F72967C-D7F3-41E2-9BA2-82E68CFB32EC}"/>
+  <autoFilter ref="A1:O2" xr:uid="{F52555E3-92DA-48AC-88C3-7AE3873D2AA6}"/>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"Non"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O1048576">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1133,20 +1161,20 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
-    <col min="4" max="4" width="57.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.81640625" style="2" customWidth="1"/>
-    <col min="8" max="9" width="12.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="86.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1178,7 +1206,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
@@ -1208,10 +1236,10 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G4" s="17"/>
     </row>
   </sheetData>
@@ -1286,16 +1314,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.453125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="91.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1338,7 @@
       </c>
       <c r="E1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1341,13 +1369,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1383,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1377,21 +1405,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="13">
-        <v>43744</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43817</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -1399,7 +1427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Ajout de grilles #42 et ajout de couleur #43
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40663D8E-D23F-4BA8-9C6F-AC1548D0C00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88DE8EC-AFE7-4127-AE33-6435C77C04C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1380" yWindow="735" windowWidth="24630" windowHeight="13710" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Général" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alertes!$A$1:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Effectifs!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alertes!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Effectifs!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Jeunes!$A$1:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -142,9 +142,6 @@
     <t>${adherent.branche}</t>
   </si>
   <si>
-    <t>Branche N+1</t>
-  </si>
-  <si>
     <t>${adherent.brancheanneeprochaine}</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     <t>&lt;jt:if test="${adherent.agecalcule}"&gt;${adherent.agecamp}&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>Branche N</t>
-  </si>
-  <si>
     <t>Droit informations OK ?</t>
   </si>
   <si>
@@ -269,6 +263,18 @@
   </si>
   <si>
     <t>Certaines colonnes contiennent des données brutes, d'autres sont calculés et parfois teintés pour indiquer un point d'attention</t>
+  </si>
+  <si>
+    <t>Branche</t>
+  </si>
+  <si>
+    <t>Branche Année+1</t>
+  </si>
+  <si>
+    <t>${alerte.adherent.branche}</t>
+  </si>
+  <si>
+    <t>${unite.branche}</t>
   </si>
 </sst>
 </file>
@@ -473,7 +479,17 @@
     <cellStyle name="Filler1" xfId="1" xr:uid="{CF299C21-B143-458E-AE9E-A0A1BA0CBE68}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -490,6 +506,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -500,6 +526,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -516,6 +562,66 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color auto="1"/>
       </font>
       <fill>
@@ -531,6 +637,56 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -904,64 +1060,64 @@
   <sheetData>
     <row r="1" spans="1:1" s="23" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -969,22 +1125,22 @@
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1023,7 +1179,7 @@
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="26" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="26" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1034,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>30</v>
@@ -1043,16 +1199,16 @@
         <v>4</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>39</v>
-      </c>
       <c r="I1" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>14</v>
@@ -1064,10 +1220,10 @@
         <v>29</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1081,25 +1237,25 @@
         <v>20</v>
       </c>
       <c r="D2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>71</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>21</v>
@@ -1111,10 +1267,10 @@
         <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q2" t="s">
         <v>0</v>
@@ -1123,25 +1279,43 @@
   </sheetData>
   <autoFilter ref="A1:O2" xr:uid="{F52555E3-92DA-48AC-88C3-7AE3873D2AA6}"/>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:J65536">
+    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+      <formula>LEFT(I2,LEN("C"))="C"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="F">
+      <formula>LEFT(I2,LEN("F"))="F"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+      <formula>LEFT(I2,LEN("PC"))="PC"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+      <formula>LEFT(I2,LEN("SG"))="SG"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+      <formula>LEFT(I2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1152,7 +1326,7 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -1169,12 +1343,13 @@
     <col min="4" max="4" width="57.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" style="2" customWidth="1"/>
-    <col min="8" max="9" width="12.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="86.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" style="2" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -1188,84 +1363,109 @@
         <v>4</v>
       </c>
       <c r="E1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="12" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" t="s">
         <v>50</v>
       </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="17"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J2" xr:uid="{5B2E4844-BE2D-4C17-93A0-1FA1B4EB5595}"/>
-  <conditionalFormatting sqref="H3:H200000">
-    <cfRule type="containsText" dxfId="5" priority="4" stopIfTrue="1" operator="containsText" text="BASSE">
-      <formula>NOT(ISERROR(SEARCH("BASSE",H3)))</formula>
+  <autoFilter ref="A1:K2" xr:uid="{5B2E4844-BE2D-4C17-93A0-1FA1B4EB5595}"/>
+  <conditionalFormatting sqref="I3:I200000">
+    <cfRule type="containsText" dxfId="15" priority="9" stopIfTrue="1" operator="containsText" text="BASSE">
+      <formula>NOT(ISERROR(SEARCH("BASSE",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H1000000">
-    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" operator="containsText" text="BASSE">
-      <formula>NOT(ISERROR(SEARCH("BASSE",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="MOYENNE">
-      <formula>NOT(ISERROR(SEARCH("MOYENNE",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" stopIfTrue="1" operator="containsText" text="HAUTE">
-      <formula>NOT(ISERROR(SEARCH("HAUTE",H2)))</formula>
+  <conditionalFormatting sqref="I2:I1000000">
+    <cfRule type="containsText" dxfId="14" priority="6" stopIfTrue="1" operator="containsText" text="BASSE">
+      <formula>NOT(ISERROR(SEARCH("BASSE",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="7" stopIfTrue="1" operator="containsText" text="MOYENNE">
+      <formula>NOT(ISERROR(SEARCH("MOYENNE",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="8" stopIfTrue="1" operator="containsText" text="HAUTE">
+      <formula>NOT(ISERROR(SEARCH("HAUTE",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G65536">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+      <formula>LEFT(G2,LEN("C"))="C"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="F">
+      <formula>LEFT(G2,LEN("F"))="F"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+      <formula>LEFT(G2,LEN("PC"))="PC"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+      <formula>LEFT(G2,LEN("SG"))="SG"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="7" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+      <formula>LEFT(G2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="6" stopIfTrue="1" operator="containsText" text="HAUTE" id="{DAF0FEC4-567C-4C8D-9922-3C0340B96299}">
+          <x14:cfRule type="containsText" priority="11" stopIfTrue="1" operator="containsText" text="HAUTE" id="{DAF0FEC4-567C-4C8D-9922-3C0340B96299}">
             <xm:f>NOT(ISERROR(SEARCH("HAUTE",Jeunes!H3)))</xm:f>
             <x14:dxf>
               <font>
@@ -1278,10 +1478,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H3:H200000</xm:sqref>
+          <xm:sqref>I3:I200000</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" stopIfTrue="1" operator="containsText" text="MOYENNE" id="{5558C640-AC39-443C-96DD-3EF988E54F02}">
+          <x14:cfRule type="containsText" priority="10" stopIfTrue="1" operator="containsText" text="MOYENNE" id="{5558C640-AC39-443C-96DD-3EF988E54F02}">
             <xm:f>NOT(ISERROR(SEARCH("MOYENNE",Jeunes!H3)))</xm:f>
             <x14:dxf>
               <font>
@@ -1294,7 +1494,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H3:H100000</xm:sqref>
+          <xm:sqref>I3:I100000</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1307,7 +1507,7 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1318,48 +1518,92 @@
   <cols>
     <col min="1" max="1" width="91.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="M2" s="1" t="s">
+      <c r="F2" s="7"/>
+      <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2" xr:uid="{6AC6ED21-E2EE-4015-ADB3-FFAFD9020971}"/>
+  <autoFilter ref="A1:E2" xr:uid="{6AC6ED21-E2EE-4015-ADB3-FFAFD9020971}"/>
+  <conditionalFormatting sqref="C2:C65536">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+      <formula>LEFT(C2,LEN("C"))="C"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+      <formula>LEFT(C2,LEN("PC"))="PC"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+      <formula>LEFT(C2,LEN("SG"))="SG"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+      <formula>LEFT(C2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="beginsWith" priority="2" stopIfTrue="1" operator="beginsWith" text="F" id="{2D57A551-1FCE-4A06-B737-1E573F7CB19A}">
+            <xm:f>LEFT(Jeunes!C2,LEN("F"))="F"</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C2:C65536</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Intégration des vents du large #54
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88DE8EC-AFE7-4127-AE33-6435C77C04C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9854377E-B3C1-4BAA-88FE-C8F2884A16A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="735" windowWidth="24630" windowHeight="13710" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="855" yWindow="1065" windowWidth="24945" windowHeight="13740" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -479,7 +479,7 @@
     <cellStyle name="Filler1" xfId="1" xr:uid="{CF299C21-B143-458E-AE9E-A0A1BA0CBE68}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="53">
     <dxf>
       <font>
         <color theme="0"/>
@@ -536,6 +536,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -546,6 +566,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -556,6 +586,16 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -566,6 +606,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
@@ -637,6 +697,226 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1279,40 +1559,43 @@
   </sheetData>
   <autoFilter ref="A1:O2" xr:uid="{F52555E3-92DA-48AC-88C3-7AE3873D2AA6}"/>
   <conditionalFormatting sqref="L2:L1048576">
-    <cfRule type="cellIs" dxfId="24" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="13" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M1048576">
-    <cfRule type="cellIs" dxfId="23" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="12" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N1048576">
-    <cfRule type="cellIs" dxfId="22" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="cellIs" dxfId="21" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Non"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:J65536">
-    <cfRule type="beginsWith" dxfId="20" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="48" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(I2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="19" priority="2" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="47" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(I2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="46" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(I2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="45" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(I2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="44" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(I2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="43" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(I2,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -1426,36 +1709,39 @@
   </sheetData>
   <autoFilter ref="A1:K2" xr:uid="{5B2E4844-BE2D-4C17-93A0-1FA1B4EB5595}"/>
   <conditionalFormatting sqref="I3:I200000">
-    <cfRule type="containsText" dxfId="15" priority="9" stopIfTrue="1" operator="containsText" text="BASSE">
+    <cfRule type="containsText" dxfId="33" priority="10" stopIfTrue="1" operator="containsText" text="BASSE">
       <formula>NOT(ISERROR(SEARCH("BASSE",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I1000000">
-    <cfRule type="containsText" dxfId="14" priority="6" stopIfTrue="1" operator="containsText" text="BASSE">
+    <cfRule type="containsText" dxfId="32" priority="7" stopIfTrue="1" operator="containsText" text="BASSE">
       <formula>NOT(ISERROR(SEARCH("BASSE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="7" stopIfTrue="1" operator="containsText" text="MOYENNE">
+    <cfRule type="containsText" dxfId="31" priority="8" stopIfTrue="1" operator="containsText" text="MOYENNE">
       <formula>NOT(ISERROR(SEARCH("MOYENNE",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="8" stopIfTrue="1" operator="containsText" text="HAUTE">
+    <cfRule type="containsText" dxfId="30" priority="9" stopIfTrue="1" operator="containsText" text="HAUTE">
       <formula>NOT(ISERROR(SEARCH("HAUTE",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G65536">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="29" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(G2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="F">
+    <cfRule type="beginsWith" dxfId="28" priority="3" stopIfTrue="1" operator="beginsWith" text="F">
       <formula>LEFT(G2,LEN("F"))="F"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="27" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(G2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="26" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(G2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="25" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(G2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="22" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(G2,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -1465,7 +1751,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="11" stopIfTrue="1" operator="containsText" text="HAUTE" id="{DAF0FEC4-567C-4C8D-9922-3C0340B96299}">
+          <x14:cfRule type="containsText" priority="12" stopIfTrue="1" operator="containsText" text="HAUTE" id="{DAF0FEC4-567C-4C8D-9922-3C0340B96299}">
             <xm:f>NOT(ISERROR(SEARCH("HAUTE",Jeunes!H3)))</xm:f>
             <x14:dxf>
               <font>
@@ -1481,7 +1767,7 @@
           <xm:sqref>I3:I200000</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" stopIfTrue="1" operator="containsText" text="MOYENNE" id="{5558C640-AC39-443C-96DD-3EF988E54F02}">
+          <x14:cfRule type="containsText" priority="11" stopIfTrue="1" operator="containsText" text="MOYENNE" id="{5558C640-AC39-443C-96DD-3EF988E54F02}">
             <xm:f>NOT(ISERROR(SEARCH("MOYENNE",Jeunes!H3)))</xm:f>
             <x14:dxf>
               <font>
@@ -1566,17 +1852,20 @@
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{6AC6ED21-E2EE-4015-ADB3-FFAFD9020971}"/>
   <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="C">
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="C">
       <formula>LEFT(C2,LEN("C"))="C"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="beginsWith" text="PC">
+    <cfRule type="beginsWith" dxfId="9" priority="4" stopIfTrue="1" operator="beginsWith" text="PC">
       <formula>LEFT(C2,LEN("PC"))="PC"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="beginsWith" text="SG">
+    <cfRule type="beginsWith" dxfId="8" priority="5" stopIfTrue="1" operator="beginsWith" text="SG">
       <formula>LEFT(C2,LEN("SG"))="SG"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="beginsWith" text="LJ">
+    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="LJ">
       <formula>LEFT(C2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="1" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(C2,LEN("V"))="V"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -1586,7 +1875,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="beginsWith" priority="2" stopIfTrue="1" operator="beginsWith" text="F" id="{2D57A551-1FCE-4A06-B737-1E573F7CB19A}">
+          <x14:cfRule type="beginsWith" priority="3" stopIfTrue="1" operator="beginsWith" text="F" id="{2D57A551-1FCE-4A06-B737-1E573F7CB19A}">
             <xm:f>LEFT(Jeunes!C2,LEN("F"))="F"</xm:f>
             <x14:dxf>
               <font>

</xml_diff>

<commit_message>
#62 Ajout d'une colonne "jeunes qui montront"
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AB5DBE-1CFB-4454-B20A-DA0CD57304DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE8B136-52E3-4592-B54F-8FA58AFD3009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="1845" yWindow="810" windowWidth="24570" windowHeight="13515" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -90,15 +90,6 @@
     <t>Marin</t>
   </si>
   <si>
-    <t>Code Unité</t>
-  </si>
-  <si>
-    <t>${unite.code}</t>
-  </si>
-  <si>
-    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="code"&gt;${unite.nom}</t>
-  </si>
-  <si>
     <t>${adherent.unite}</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>&lt;jt:if test="${adherent.marin}"&gt;Oui&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${adherents}" var="adherent" where="${adherent.jeune == 1}" orderBy="fonction;unite;nom"&gt;${adherent.code}</t>
-  </si>
-  <si>
     <t>Age année OK ?</t>
   </si>
   <si>
@@ -277,6 +265,18 @@
   </si>
   <si>
     <t>Feuille "Alertes"</t>
+  </si>
+  <si>
+    <t>Montées Année N+1</t>
+  </si>
+  <si>
+    <t>${unite.montees}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${unites}" var="unite" orderBy="tribranche"&gt;${unite.nom}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${adherents}" var="adherent" where="${adherent.jeune == 1}" orderBy="tribranche;unite;nom"&gt;${adherent.code}</t>
   </si>
 </sst>
 </file>
@@ -496,67 +496,67 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1110,64 +1110,64 @@
   <sheetData>
     <row r="1" spans="1:1" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1175,22 +1175,22 @@
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1240,87 +1240,87 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="25" t="s">
+      <c r="M2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>36</v>
-      </c>
       <c r="O2" s="20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="P2" s="20"/>
       <c r="Q2" s="21" t="s">
@@ -1417,58 +1417,58 @@
         <v>4</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="J1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L2" s="27"/>
     </row>
@@ -1575,25 +1575,25 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="4.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>5</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>6</v>
@@ -1602,16 +1602,16 @@
     </row>
     <row r="2" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="25" t="s">
         <v>76</v>
       </c>
+      <c r="B2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="28" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>7</v>
@@ -1623,27 +1623,27 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{6AC6ED21-E2EE-4015-ADB3-FFAFD9020971}"/>
-  <conditionalFormatting sqref="C2:C65536">
-    <cfRule type="beginsWith" dxfId="6" priority="3" stopIfTrue="1" operator="beginsWith" text="SG">
-      <formula>LEFT(C2,LEN("SG"))="SG"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="4" stopIfTrue="1" operator="beginsWith" text="C">
-      <formula>LEFT(C2,LEN("C"))="C"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="5" stopIfTrue="1" operator="beginsWith" text="F">
-      <formula>LEFT(C2,LEN("F"))="F"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="6" stopIfTrue="1" operator="beginsWith" text="V">
-      <formula>LEFT(C2,LEN("V"))="V"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="7" stopIfTrue="1" operator="beginsWith" text="R">
-      <formula>LEFT(C2,LEN("R"))="R"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="LJ">
-      <formula>LEFT(C2,LEN("LJ"))="LJ"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="beginsWith" text="PC">
-      <formula>LEFT(C2,LEN("PC"))="PC"</formula>
+  <conditionalFormatting sqref="B2:B65536">
+    <cfRule type="beginsWith" dxfId="6" priority="1" stopIfTrue="1" operator="beginsWith" text="PC">
+      <formula>LEFT(B2,LEN("PC"))="PC"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="LJ">
+      <formula>LEFT(B2,LEN("LJ"))="LJ"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="3" stopIfTrue="1" operator="beginsWith" text="SG">
+      <formula>LEFT(B2,LEN("SG"))="SG"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="4" stopIfTrue="1" operator="beginsWith" text="C">
+      <formula>LEFT(B2,LEN("C"))="C"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="5" stopIfTrue="1" operator="beginsWith" text="F">
+      <formula>LEFT(B2,LEN("F"))="F"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="6" stopIfTrue="1" operator="beginsWith" text="V">
+      <formula>LEFT(B2,LEN("V"))="V"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="beginsWith" text="R">
+      <formula>LEFT(B2,LEN("R"))="R"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1" gridLines="1"/>
@@ -1666,10 +1666,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="8">
-        <v>43967</v>
+        <v>43985</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,10 +1718,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#70 Ajout des pré-inscrits jeunes, compas et farfadets
</commit_message>
<xml_diff>
--- a/fichiers/conf/modele_jeunes.xlsx
+++ b/fichiers/conf/modele_jeunes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\analytiscout\fichiers\conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE8B136-52E3-4592-B54F-8FA58AFD3009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B852D4-8FA0-4018-9680-4433FCBA5632}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="810" windowWidth="24570" windowHeight="13515" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
+    <workbookView xWindow="225" yWindow="90" windowWidth="25080" windowHeight="14745" tabRatio="391" activeTab="1" xr2:uid="{65826371-4A86-45E5-8D4B-7C8F7979A5BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Aide" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>&lt;/jt:forEach&gt;</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${adherents}" var="adherent" where="${adherent.jeune == 1}" orderBy="tribranche;unite;nom"&gt;${adherent.code}</t>
+  </si>
+  <si>
+    <t>${adherent.typeadhesion}</t>
+  </si>
+  <si>
+    <t>Type adhésion</t>
   </si>
 </sst>
 </file>
@@ -286,7 +292,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,8 +368,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +386,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDABE5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,7 +426,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,6 +503,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Filler1" xfId="1" xr:uid="{CF299C21-B143-458E-AE9E-A0A1BA0CBE68}"/>
@@ -1204,11 +1229,13 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,10 +1253,12 @@
     <col min="11" max="11" width="8" style="1" customWidth="1"/>
     <col min="12" max="14" width="11" style="1" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="19" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="19" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1275,8 +1304,12 @@
       <c r="O1" s="13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P1"/>
+      <c r="Q1" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>77</v>
       </c>
@@ -1322,10 +1355,17 @@
       <c r="O2" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21" t="s">
+      <c r="P2" s="30"/>
+      <c r="Q2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="21" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O2" xr:uid="{F52555E3-92DA-48AC-88C3-7AE3873D2AA6}"/>

</xml_diff>